<commit_message>
adding Telangana and Andhra
</commit_message>
<xml_diff>
--- a/Vadodara Hospitals.xlsx
+++ b/Vadodara Hospitals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K249"/>
+  <dimension ref="A1:K259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9450,26 +9450,22 @@
         </is>
       </c>
       <c r="D185" t="n">
-        <v>22.3044244</v>
+        <v>22.3029368</v>
       </c>
       <c r="E185" t="n">
-        <v>73.15507389999999</v>
+        <v>73.1532313</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>ChIJqcDxBpnIXzkRKanH1j2ldOI</t>
+          <t>ChIJA88FsoTJXzkR5SzSqXxRoHk</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=Prisha+Hospital&amp;query_place_id=ChIJqcDxBpnIXzkRKanH1j2ldOI</t>
-        </is>
-      </c>
-      <c r="H185" t="inlineStr">
-        <is>
-          <t>0265 233 3232</t>
-        </is>
-      </c>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Prisha+Hospital+Dr+Jayesh+Solanki&amp;query_place_id=ChIJA88FsoTJXzkR5SzSqXxRoHk</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr"/>
       <c r="I185" t="inlineStr">
         <is>
           <t>Dr. Ashish Lakkad</t>
@@ -12331,10 +12327,22 @@
           <t>Samras Hostel (Extension of SSG Hospital), Polytechnic, University Campus</t>
         </is>
       </c>
-      <c r="D243" t="inlineStr"/>
-      <c r="E243" t="inlineStr"/>
-      <c r="F243" t="inlineStr"/>
-      <c r="G243" t="inlineStr"/>
+      <c r="D243" t="n">
+        <v>22.34301</v>
+      </c>
+      <c r="E243" t="n">
+        <v>73.1951727</v>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>ChIJ63rXNibPXzkRWBhO48yxgpo</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Samras+Boy%27s+Hostel&amp;query_place_id=ChIJ63rXNibPXzkRWBhO48yxgpo</t>
+        </is>
+      </c>
       <c r="H243" t="inlineStr"/>
       <c r="I243" t="inlineStr">
         <is>
@@ -12457,44 +12465,44 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Community Health Centre Padra</t>
+          <t>Pioneer Campus ICU (Extension Facility of Sunshine Global Hospital)</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Near New ST Depot, Jambusar Road, Padra</t>
+          <t>Sayajipura, Ajwa road</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Community Health Centre Padra, Near New ST Depot, Jambusar Road, Padra</t>
+          <t>Pioneer Campus ICU (Extension Facility of Sunshine Global Hospital), Sayajipura, Ajwa road</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>22.2457969</v>
+        <v>22.3273678</v>
       </c>
       <c r="E246" t="n">
-        <v>73.084673</v>
+        <v>73.2634284</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>ChIJbaStAn-4XzkRfHkNU4hDX3s</t>
+          <t>ChIJb06ca_PPXzkRyJK8H5n-UgM</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=Community+Health+Centre+Padra&amp;query_place_id=ChIJbaStAn-4XzkRfHkNU4hDX3s</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Pioneer+Homoeopathic+Medical+College+&amp;+Hospital&amp;query_place_id=ChIJb06ca_PPXzkRyJK8H5n-UgM</t>
         </is>
       </c>
       <c r="H246" t="inlineStr"/>
       <c r="I246" t="inlineStr">
         <is>
-          <t>Dr. Meena Agaja</t>
+          <t>Mr. Kaushal Panchal</t>
         </is>
       </c>
       <c r="J246" t="inlineStr">
         <is>
-          <t>7990162366</t>
+          <t>9558945191</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -12506,44 +12514,44 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Singh Urology Hospital</t>
+          <t>Community Health Centre Padra</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Pancham Icon, Opp.Ajwa Water tank, Sardar Estate, New VIP Road</t>
+          <t>Near New ST Depot, Jambusar Road, Padra</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Singh Urology Hospital, Pancham Icon, Opp.Ajwa Water tank, Sardar Estate, New VIP Road</t>
+          <t>Community Health Centre Padra, Near New ST Depot, Jambusar Road, Padra</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>22.3138741</v>
+        <v>22.1589887</v>
       </c>
       <c r="E247" t="n">
-        <v>73.2335748</v>
+        <v>72.93429449999999</v>
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>ChIJ2bLCjJ_PXzkRrYnqmFZQFto</t>
+          <t>ChIJCZA7uoe4XzkRxNW3t4SJz7g</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=Singh+Urology+Hospital&amp;query_place_id=ChIJ2bLCjJ_PXzkRrYnqmFZQFto</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Community+Health+Centre+Padra&amp;query_place_id=ChIJCZA7uoe4XzkRxNW3t4SJz7g</t>
         </is>
       </c>
       <c r="H247" t="inlineStr"/>
       <c r="I247" t="inlineStr">
         <is>
-          <t>Dr. Dhaval Pithwa</t>
+          <t>Dr. Meena Agaja</t>
         </is>
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>9773423968</t>
+          <t>7990162366</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -12555,48 +12563,44 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Akshar Hospital (Extension of Shreeji Hospital, Maneja)</t>
+          <t>Pioneer Campus (Managed by Singhania Dental &amp; ENT Care)</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Patidar Complex, Por. Ta. Vadodara</t>
+          <t>Sayajipura, Ajwa road</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Akshar Hospital (Extension of Shreeji Hospital, Maneja), Patidar Complex, Por. Ta. Vadodara</t>
+          <t>Pioneer Campus (Managed by Singhania Dental &amp; ENT Care), Sayajipura, Ajwa road</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>22.2396503</v>
+        <v>22.3273678</v>
       </c>
       <c r="E248" t="n">
-        <v>73.1882423</v>
+        <v>73.2634284</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>ChIJG2tgIiTEXzkRO4lfKr4XzMo</t>
+          <t>ChIJb06ca_PPXzkRyJK8H5n-UgM</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=Akshar+Hospital+(Extension+of+Shreeji+Hospital,+Maneja)&amp;query_place_id=ChIJG2tgIiTEXzkRO4lfKr4XzMo</t>
-        </is>
-      </c>
-      <c r="H248" t="inlineStr">
-        <is>
-          <t>098255 56885</t>
-        </is>
-      </c>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Pioneer+Homoeopathic+Medical+College+&amp;+Hospital&amp;query_place_id=ChIJb06ca_PPXzkRyJK8H5n-UgM</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr"/>
       <c r="I248" t="inlineStr">
         <is>
-          <t>Dr. Upesh Parmar</t>
+          <t>Dr. Ankit Singhania</t>
         </is>
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>9099922964</t>
+          <t>9426530739</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -12608,51 +12612,545 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>NAMO Covid Isolation Center</t>
+          <t>Singh Urology Hospital</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
+          <t>Pancham Icon, Opp.Ajwa Water tank, Sardar Estate, New VIP Road</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Singh Urology Hospital, Pancham Icon, Opp.Ajwa Water tank, Sardar Estate, New VIP Road</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>22.3138741</v>
+      </c>
+      <c r="E249" t="n">
+        <v>73.2335748</v>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>ChIJ2bLCjJ_PXzkRrYnqmFZQFto</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Singh+Urology+Hospital&amp;query_place_id=ChIJ2bLCjJ_PXzkRrYnqmFZQFto</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr"/>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>Dr. Dhaval Pithwa</t>
+        </is>
+      </c>
+      <c r="J249" t="inlineStr">
+        <is>
+          <t>9773423968</t>
+        </is>
+      </c>
+      <c r="K249" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Akshar Hospital (Extension of Shreeji Hospital, Maneja)</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Patidar Complex, Por. Ta. Vadodara</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Akshar Hospital (Extension of Shreeji Hospital, Maneja), Patidar Complex, Por. Ta. Vadodara</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>22.2396503</v>
+      </c>
+      <c r="E250" t="n">
+        <v>73.1882423</v>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>ChIJG2tgIiTEXzkRO4lfKr4XzMo</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Akshar+Hospital+(Extension+of+Shreeji+Hospital,+Maneja)&amp;query_place_id=ChIJG2tgIiTEXzkRO4lfKr4XzMo</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>098255 56885</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>Dr. Upesh Parmar</t>
+        </is>
+      </c>
+      <c r="J250" t="inlineStr">
+        <is>
+          <t>9099922964</t>
+        </is>
+      </c>
+      <c r="K250" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Ayushya Hospital (Unit of Unity Hospital, Vadsar)</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Dorado Complex, Rajnikant Jani Road, Relience Circle, Opp Shreyas School, Manjalpur, Vadodara</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Ayushya Hospital (Unit of Unity Hospital, Vadsar), Dorado Complex, Rajnikant Jani Road, Relience Circle, Opp Shreyas School, Manjalpur, Vadodara</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>22.2771068</v>
+      </c>
+      <c r="E251" t="n">
+        <v>73.1978372</v>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>ChIJRRhd3-nFXzkRVDEltAm5gXE</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Ayushya+Hospital+(Unit+of+Unity+Hospital,+Vadsar)&amp;query_place_id=ChIJRRhd3-nFXzkRVDEltAm5gXE</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>0265 263 2189</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>Dr. Rushik Kaneriya</t>
+        </is>
+      </c>
+      <c r="J251" t="inlineStr">
+        <is>
+          <t>8000428343</t>
+        </is>
+      </c>
+      <c r="K251" t="inlineStr">
+        <is>
+          <t>Savita Cluster</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Aziz Hospital</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>New Heaven Enclave, Near Harish Patrol Pump, Panigate</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Aziz Hospital, New Heaven Enclave, Near Harish Patrol Pump, Panigate</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>22.2994653</v>
+      </c>
+      <c r="E252" t="n">
+        <v>73.22014899999999</v>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>ChIJuUbP2KzIXzkRHlLssyI4ZTw</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Aziz+Hospital&amp;query_place_id=ChIJuUbP2KzIXzkRHlLssyI4ZTw</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>0265 256 1342</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>Dr. Murtaza</t>
+        </is>
+      </c>
+      <c r="J252" t="inlineStr">
+        <is>
+          <t>9428507862</t>
+        </is>
+      </c>
+      <c r="K252" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>NAMO Covid Isolation Care Center</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Milan Party Plot Hall New VIP Road, Vadodara</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>NAMO Covid Isolation Care Center, Milan Party Plot Hall New VIP Road, Vadodara</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>22.3258391</v>
+      </c>
+      <c r="E253" t="n">
+        <v>73.21801959999999</v>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>ChIJ4b9ZVA3PXzkRiL4xksen7xM</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=NAMO+Covid+Isolation+Care+Center&amp;query_place_id=ChIJ4b9ZVA3PXzkRiL4xksen7xM</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr"/>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>Dr. Krutik M. Majithiya</t>
+        </is>
+      </c>
+      <c r="J253" t="inlineStr">
+        <is>
+          <t>8264000239</t>
+        </is>
+      </c>
+      <c r="K253" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>NAMO Covid-19 Isolation Facility</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
           <t>My Shannen School, Near Mukinagar, Khodiyarnagar, New VIP Road</t>
         </is>
       </c>
-      <c r="C249" t="inlineStr">
-        <is>
-          <t>NAMO Covid Isolation Center, My Shannen School, Near Mukinagar, Khodiyarnagar, New VIP Road</t>
-        </is>
-      </c>
-      <c r="D249" t="n">
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>NAMO Covid-19 Isolation Facility, My Shannen School, Near Mukinagar, Khodiyarnagar, New VIP Road</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
         <v>22.3221439</v>
       </c>
-      <c r="E249" t="n">
+      <c r="E254" t="n">
         <v>73.23354359999999</v>
       </c>
-      <c r="F249" t="inlineStr">
+      <c r="F254" t="inlineStr">
         <is>
           <t>ChIJdRoQmZ7PXzkRjVYkFSshTHw</t>
         </is>
       </c>
-      <c r="G249" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=NAMO+Covid+Isolation+Center&amp;query_place_id=ChIJdRoQmZ7PXzkRjVYkFSshTHw</t>
-        </is>
-      </c>
-      <c r="H249" t="inlineStr">
-        <is>
-          <t>081550 55093</t>
-        </is>
-      </c>
-      <c r="I249" t="inlineStr">
-        <is>
-          <t>Dr. Uvraj Sisodiya</t>
-        </is>
-      </c>
-      <c r="J249" t="inlineStr">
-        <is>
-          <t>8141617498</t>
-        </is>
-      </c>
-      <c r="K249" t="inlineStr">
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=NAMO+Covid-19+Isolation+Facility&amp;query_place_id=ChIJdRoQmZ7PXzkRjVYkFSshTHw</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr"/>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>Mehul Patel</t>
+        </is>
+      </c>
+      <c r="J254" t="inlineStr">
+        <is>
+          <t>8238936352</t>
+        </is>
+      </c>
+      <c r="K254" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Atri Sushrusha Hospital &amp; ICU (Extension of Dev Hospital &amp; ICU, Tarsali)</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Timbarva, Ta. Sinor</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Atri Sushrusha Hospital &amp; ICU (Extension of Dev Hospital &amp; ICU, Tarsali), Timbarva, Ta. Sinor</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>22</v>
+      </c>
+      <c r="E255" t="n">
+        <v>73</v>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>ChIJK9QDSsfFXzkRQFS1Wo8f_4M</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Atri+Sushrusha+Hospital+&amp;+ICU+(Extension+of+Dev+Hospital+&amp;+ICU,+Tarsali)&amp;query_place_id=ChIJK9QDSsfFXzkRQFS1Wo8f_4M</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr"/>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>Dr. Keyur Bamaniya</t>
+        </is>
+      </c>
+      <c r="J255" t="inlineStr">
+        <is>
+          <t>9664546829</t>
+        </is>
+      </c>
+      <c r="K255" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Lalwani Hospital</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Meera Society, Near Rajiv nagar-2, Diwalipura Main road</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Lalwani Hospital, Meera Society, Near Rajiv nagar-2, Diwalipura Main road</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>22</v>
+      </c>
+      <c r="E256" t="n">
+        <v>73</v>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>ChIJZRLgl57IXzkRqKjYD9tM-04</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Lalwani+Hospital&amp;query_place_id=ChIJZRLgl57IXzkRqKjYD9tM-04</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr"/>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>Dr. Prasanna Lalwani</t>
+        </is>
+      </c>
+      <c r="J256" t="inlineStr">
+        <is>
+          <t>9998485950</t>
+        </is>
+      </c>
+      <c r="K256" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Shashwat Hospital - Salatwada</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Beside Bombay Mercantile bank, Kothi Salatwada Road</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Shashwat Hospital - Salatwada, Beside Bombay Mercantile bank, Kothi Salatwada Road</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>22</v>
+      </c>
+      <c r="E257" t="n">
+        <v>73</v>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>ChIJAQAA0FvPXzkR09_CgRN1Ebs</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Shashwat+Hospital+-+Salatwada&amp;query_place_id=ChIJAQAA0FvPXzkR09_CgRN1Ebs</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>0265 242 4276</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>Dr. Shrenik Vaidya</t>
+        </is>
+      </c>
+      <c r="J257" t="inlineStr">
+        <is>
+          <t>9824023251</t>
+        </is>
+      </c>
+      <c r="K257" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Shrinathji Hospital - Sakuntal Complex</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Near Kaladarshan Char rasta, Waghodiya Road</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Shrinathji Hospital - Sakuntal Complex, Near Kaladarshan Char rasta, Waghodiya Road</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>22</v>
+      </c>
+      <c r="E258" t="n">
+        <v>73</v>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>ChIJmc1ADnjFXzkR29eDYsqyF5g</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=Shrinathji+Hospital+-+Sakuntal+Complex&amp;query_place_id=ChIJmc1ADnjFXzkR29eDYsqyF5g</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr"/>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>Dr. Meena Shah</t>
+        </is>
+      </c>
+      <c r="J258" t="inlineStr">
+        <is>
+          <t>9104516383</t>
+        </is>
+      </c>
+      <c r="K258" t="inlineStr">
+        <is>
+          <t>Not Define</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Srijan Hospital</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Shop 18-25, Third Floor, Corner point, Maneja</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Srijan Hospital, Shop 18-25, Third Floor, Corner point, Maneja</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>0</v>
+      </c>
+      <c r="E259" t="n">
+        <v>0</v>
+      </c>
+      <c r="F259" t="inlineStr"/>
+      <c r="G259" t="inlineStr"/>
+      <c r="H259" t="inlineStr"/>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>Dr. Vishalkumar Thakur</t>
+        </is>
+      </c>
+      <c r="J259" t="inlineStr">
+        <is>
+          <t>7045536141</t>
+        </is>
+      </c>
+      <c r="K259" t="inlineStr">
         <is>
           <t>Not Define</t>
         </is>

</xml_diff>